<commit_message>
docs: adjust column width of colJ
</commit_message>
<xml_diff>
--- a/mugna/assets/basis.xlsx
+++ b/mugna/assets/basis.xlsx
@@ -8,19 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\repos\Mugna\mugna\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB603A7-8238-4DB2-BC92-7E0490EC0230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6DCC9D-39A7-4A55-92B4-08A34C8AF98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V44"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -452,18 +448,18 @@
     <col min="5" max="6" width="22.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="0.85546875" style="5" customWidth="1"/>
     <col min="8" max="9" width="22.7109375" style="5" customWidth="1"/>
-    <col min="10" max="12" width="0.85546875" style="5" customWidth="1"/>
-    <col min="13" max="14" width="22.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="0.85546875" style="5" customWidth="1"/>
-    <col min="16" max="17" width="22.7109375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="0.85546875" style="5" customWidth="1"/>
-    <col min="19" max="20" width="22.7109375" style="5" customWidth="1"/>
-    <col min="21" max="22" width="0.85546875" style="5" customWidth="1"/>
-    <col min="23" max="48" width="9.140625" style="5" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="5"/>
+    <col min="10" max="11" width="0.85546875" style="5" customWidth="1"/>
+    <col min="12" max="13" width="22.7109375" style="5" customWidth="1"/>
+    <col min="14" max="14" width="0.85546875" style="5" customWidth="1"/>
+    <col min="15" max="16" width="22.7109375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="0.85546875" style="5" customWidth="1"/>
+    <col min="18" max="19" width="22.7109375" style="5" customWidth="1"/>
+    <col min="20" max="21" width="0.85546875" style="5" customWidth="1"/>
+    <col min="22" max="47" width="9.140625" style="5" customWidth="1"/>
+    <col min="48" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="4"/>
@@ -476,18 +472,17 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="4"/>
       <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:22" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:21" s="8" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -499,19 +494,18 @@
       <c r="I2" s="7"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="7"/>
       <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="T2" s="6"/>
       <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-    </row>
-    <row r="3" spans="1:22" s="8" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:21" s="8" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -523,19 +517,18 @@
       <c r="I3" s="7"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="T3" s="6"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-    </row>
-    <row r="4" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -546,18 +539,17 @@
       <c r="H4" s="4"/>
       <c r="I4" s="2"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="2"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="1"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="2"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4"/>
@@ -570,18 +562,17 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="4"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4"/>
@@ -594,18 +585,17 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="4"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4"/>
@@ -618,18 +608,17 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="4"/>
       <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
+      <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="10"/>
@@ -642,18 +631,17 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="3"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="10"/>
@@ -666,18 +654,17 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="3"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="10"/>
@@ -690,18 +677,17 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="3"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="10"/>
@@ -714,18 +700,17 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="3"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4"/>
@@ -736,16 +721,15 @@
       <c r="J12" s="9"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="1"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="9"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="1"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -757,19 +741,18 @@
       <c r="I13" s="14"/>
       <c r="J13" s="9"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+      <c r="L13" s="11"/>
       <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="1"/>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="4"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -781,17 +764,16 @@
       <c r="J14" s="9"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="1"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="2"/>
+      <c r="Q14" s="1"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -803,17 +785,16 @@
       <c r="J15" s="9"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="4"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="2"/>
+      <c r="N15" s="4"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -824,16 +805,15 @@
       <c r="J16" s="9"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="4"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T16" s="9"/>
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -846,18 +826,17 @@
       <c r="J17" s="9"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3"/>
@@ -870,18 +849,17 @@
       <c r="J18" s="9"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="9"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T18" s="9"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="3"/>
@@ -894,18 +872,17 @@
       <c r="J19" s="9"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="4"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T19" s="9"/>
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="3"/>
@@ -918,18 +895,17 @@
       <c r="J20" s="9"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T20" s="9"/>
+      <c r="U20" s="1"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="4"/>
@@ -942,65 +918,60 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+      <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
+      <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="1:22" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="1"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
+      <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="1"/>
-    </row>
-    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+      <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
+      <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-    </row>
-    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="4"/>
@@ -1012,16 +983,15 @@
       <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="1"/>
-    </row>
-    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N26" s="1"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="1"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="4"/>
@@ -1033,16 +1003,15 @@
       <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="1"/>
-    </row>
-    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N27" s="1"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="1"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="4"/>
@@ -1054,16 +1023,15 @@
       <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N28" s="1"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="4"/>
@@ -1075,16 +1043,15 @@
       <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="1"/>
-    </row>
-    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N29" s="1"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="1"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="4"/>
@@ -1096,16 +1063,15 @@
       <c r="I30" s="4"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N30" s="1"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="4"/>
@@ -1117,16 +1083,15 @@
       <c r="I31" s="4"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N31" s="1"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="1"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="4"/>
@@ -1138,16 +1103,15 @@
       <c r="I32" s="4"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="1"/>
-    </row>
-    <row r="33" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N32" s="1"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="1"/>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="4"/>
@@ -1159,16 +1123,15 @@
       <c r="I33" s="4"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
+      <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="1"/>
-    </row>
-    <row r="34" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N33" s="1"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="4"/>
@@ -1180,16 +1143,15 @@
       <c r="I34" s="4"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+      <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="1"/>
-    </row>
-    <row r="35" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N34" s="1"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="4"/>
@@ -1201,16 +1163,15 @@
       <c r="I35" s="4"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="L35" s="4"/>
       <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="1"/>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N35" s="1"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="4"/>
@@ -1222,16 +1183,15 @@
       <c r="I36" s="4"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
+      <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="4"/>
-      <c r="S36" s="1"/>
-    </row>
-    <row r="37" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N36" s="1"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="4"/>
@@ -1243,16 +1203,15 @@
       <c r="I37" s="4"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="L37" s="4"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="4"/>
-      <c r="S37" s="1"/>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N37" s="1"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="4"/>
@@ -1264,16 +1223,15 @@
       <c r="I38" s="4"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="L38" s="4"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="4"/>
-      <c r="S38" s="1"/>
-    </row>
-    <row r="39" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N38" s="1"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="4"/>
@@ -1285,16 +1243,15 @@
       <c r="I39" s="4"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="1"/>
-    </row>
-    <row r="40" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N39" s="1"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="1"/>
+    </row>
+    <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="4"/>
@@ -1306,16 +1263,15 @@
       <c r="I40" s="4"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="1"/>
-    </row>
-    <row r="41" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N40" s="1"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="4"/>
@@ -1327,16 +1283,15 @@
       <c r="I41" s="4"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
+      <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="4"/>
-      <c r="S41" s="1"/>
-    </row>
-    <row r="42" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N41" s="1"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="1"/>
+    </row>
+    <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="4"/>
@@ -1348,16 +1303,15 @@
       <c r="I42" s="4"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="1"/>
-    </row>
-    <row r="43" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N42" s="1"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="1"/>
+    </row>
+    <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1376,9 +1330,8 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-    </row>
-    <row r="44" spans="1:19" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="4"/>
@@ -1390,14 +1343,13 @@
       <c r="I44" s="4"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
+      <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>